<commit_message>
Ultrasonic sensor calibration experiments
</commit_message>
<xml_diff>
--- a/Doc/Servo.xlsx
+++ b/Doc/Servo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fermartv\Google Drive\5. Ideas\Picar-S\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.138\Raspi compartida\Pruebas Picar\My robot\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE9A591-7E28-45E5-B069-4FC2404EFBD0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F579C062-3B89-4220-A8B4-E327F6C4FDB3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{56478B2C-2DF0-43D5-8170-BB6F25C80C1F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{56478B2C-2DF0-43D5-8170-BB6F25C80C1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>micro s</t>
   </si>
@@ -95,14 +95,20 @@
   <si>
     <t>Hz</t>
   </si>
+  <si>
+    <t>Calculated Duty cycle</t>
+  </si>
+  <si>
+    <t>Calculated Duty cycle (12-bits)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="175" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -150,8 +156,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,8 +756,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
@@ -768,18 +774,72 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$K$2:$K$38</c:f>
               <c:numCache>
@@ -898,8 +958,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Hoja1!$N$2:$N$38</c:f>
               <c:numCache>
@@ -1018,7 +1078,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1034,11 +1094,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="617493167"/>
         <c:axId val="584795807"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="617493167"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1084,11 +1143,8 @@
         </c:txPr>
         <c:crossAx val="584795807"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="584795807"/>
         <c:scaling>
@@ -1143,7 +1199,7 @@
         </c:txPr>
         <c:crossAx val="617493167"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1298,8 +1354,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1316,18 +1372,72 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$L$2:$L$38</c:f>
               <c:numCache>
@@ -1446,8 +1556,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Hoja1!$N$2:$N$38</c:f>
               <c:numCache>
@@ -1566,7 +1676,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1582,11 +1692,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="584216799"/>
         <c:axId val="447866959"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="584216799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1632,11 +1741,8 @@
         </c:txPr>
         <c:crossAx val="447866959"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="447866959"/>
         <c:scaling>
@@ -1691,7 +1797,7 @@
         </c:txPr>
         <c:crossAx val="584216799"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3446,16 +3552,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>445407</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>77107</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>90714</xdr:rowOff>
+      <xdr:rowOff>122464</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>445407</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>167821</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>77107</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>15421</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3482,16 +3588,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>170089</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>55789</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>138792</xdr:rowOff>
+      <xdr:rowOff>145142</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>170089</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>55789</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>48532</xdr:rowOff>
+      <xdr:rowOff>54882</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3816,10 +3922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6CAE20-962B-46A1-B1D2-A90F2A2465E3}">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3830,7 +3936,7 @@
     <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3864,8 +3970,14 @@
       <c r="N1" t="s">
         <v>9</v>
       </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3880,7 +3992,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <f>(E2-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
+        <f t="shared" ref="F2:F14" si="0">(E2-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
         <v>600</v>
       </c>
       <c r="G2" s="2">
@@ -3902,15 +4014,19 @@
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="N2">
-        <f>TRUNC(M2*4096,0)</f>
+        <f t="shared" ref="N2:N38" si="1">TRUNC(M2*4096,0)</f>
         <v>147</v>
       </c>
       <c r="O2" s="3">
-        <f>($B$7-$B$6)/$B$2*L2+$B$7-$B$7/2-$B$6/2</f>
-        <v>0</v>
+        <f>($B$6-$B$7)/-180*L2+$B$7+($B$6-$B$7)/2</f>
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="P2">
+        <f>TRUNC(O2*4096,0)</f>
+        <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3926,15 +4042,15 @@
         <v>15</v>
       </c>
       <c r="F3">
-        <f>(E3-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
+        <f t="shared" si="0"/>
         <v>750</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G14" si="0">TRUNC(F3,0)/1000000*60</f>
+        <f t="shared" ref="G3:G14" si="2">TRUNC(F3,0)/1000000*60</f>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H14" si="1">TRUNC(TRUNC(F3,0)/1000000*60*4096,0)</f>
+        <f t="shared" ref="H3:H14" si="3">TRUNC(TRUNC(F3,0)/1000000*60*4096,0)</f>
         <v>184</v>
       </c>
       <c r="K3">
@@ -3946,15 +4062,23 @@
         <v>-85</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M38" si="2">($B$7-$B$6)/$B$2*L3+$B$7-($B$7-$B$6)/2</f>
+        <f t="shared" ref="M3:M38" si="4">($B$7-$B$6)/$B$2*L3+$B$7-($B$7-$B$6)/2</f>
         <v>3.9000000000000007E-2</v>
       </c>
       <c r="N3">
-        <f>TRUNC(M3*4096,0)</f>
+        <f t="shared" si="1"/>
         <v>159</v>
       </c>
+      <c r="O3" s="3">
+        <f t="shared" ref="O3:O38" si="5">($B$6-$B$7)/-180*L3+$B$7+($B$6-$B$7)/2</f>
+        <v>3.9000000000000007E-2</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P38" si="6">TRUNC(O3*4096,0)</f>
+        <v>159</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3966,39 +4090,47 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4">
-        <f t="shared" ref="E4:E14" si="3">E3+15</f>
+        <f t="shared" ref="E4:E14" si="7">E3+15</f>
         <v>30</v>
       </c>
       <c r="F4">
-        <f>(E4-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
+        <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="H4" s="1">
+        <f t="shared" si="3"/>
+        <v>221</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K37" si="8">K3+5</f>
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L37" si="9">L3+5</f>
+        <v>-80</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>4.200000000000001E-2</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="1"/>
-        <v>221</v>
-      </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K37" si="4">K3+5</f>
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L37" si="5">L3+5</f>
-        <v>-80</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="5"/>
         <v>4.200000000000001E-2</v>
       </c>
-      <c r="N4">
-        <f>TRUNC(M4*4096,0)</f>
+      <c r="P4">
+        <f t="shared" si="6"/>
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -4010,39 +4142,47 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1050</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="2"/>
+        <v>6.3E-2</v>
+      </c>
+      <c r="H5" s="1">
         <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="F5">
-        <f>(E5-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>1050</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>6.3E-2</v>
-      </c>
-      <c r="H5" s="1">
+        <v>258</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="9"/>
+        <v>-75</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="1"/>
-        <v>258</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="L5">
+        <v>184</v>
+      </c>
+      <c r="O5" s="3">
         <f t="shared" si="5"/>
-        <v>-75</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="N5">
-        <f>TRUNC(M5*4096,0)</f>
+      <c r="P5">
+        <f t="shared" si="6"/>
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4052,39 +4192,47 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="H6" s="1">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="F6">
-        <f>(E6-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>1200</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="H6" s="1">
+        <v>294</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="9"/>
+        <v>-70</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="1"/>
-        <v>294</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="L6">
+        <v>196</v>
+      </c>
+      <c r="O6" s="3">
         <f t="shared" si="5"/>
-        <v>-70</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="2"/>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="N6">
-        <f>TRUNC(M6*4096,0)</f>
+      <c r="P6">
+        <f t="shared" si="6"/>
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4094,772 +4242,1020 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1350</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="H7" s="1">
         <f t="shared" si="3"/>
-        <v>75</v>
-      </c>
-      <c r="F7">
-        <f>(E7-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>1350</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="H7" s="1">
+        <v>331</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="9"/>
+        <v>-65</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>5.099999999999999E-2</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="1"/>
-        <v>331</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
-      <c r="L7">
+        <v>208</v>
+      </c>
+      <c r="O7" s="3">
         <f t="shared" si="5"/>
-        <v>-65</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="2"/>
         <v>5.099999999999999E-2</v>
       </c>
-      <c r="N7">
-        <f>TRUNC(M7*4096,0)</f>
+      <c r="P7">
+        <f t="shared" si="6"/>
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D8" s="1"/>
       <c r="E8">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.09</v>
+      </c>
+      <c r="H8" s="1">
         <f t="shared" si="3"/>
-        <v>90</v>
-      </c>
-      <c r="F8">
-        <f>(E8-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>1500</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.09</v>
-      </c>
-      <c r="H8" s="1">
+        <v>368</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="9"/>
+        <v>-60</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>5.3999999999999992E-2</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="1"/>
-        <v>368</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="L8">
+        <v>221</v>
+      </c>
+      <c r="O8" s="3">
         <f t="shared" si="5"/>
-        <v>-60</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="2"/>
         <v>5.3999999999999992E-2</v>
       </c>
-      <c r="N8">
-        <f>TRUNC(M8*4096,0)</f>
+      <c r="P8">
+        <f t="shared" si="6"/>
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D9" s="1"/>
       <c r="E9">
+        <f t="shared" si="7"/>
+        <v>105</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1650</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="H9" s="1">
         <f t="shared" si="3"/>
-        <v>105</v>
-      </c>
-      <c r="F9">
-        <f>(E9-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>1650</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="H9" s="1">
+        <v>405</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="9"/>
+        <v>-55</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>5.6999999999999995E-2</v>
+      </c>
+      <c r="N9">
         <f t="shared" si="1"/>
-        <v>405</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="4"/>
-        <v>35</v>
-      </c>
-      <c r="L9">
+        <v>233</v>
+      </c>
+      <c r="O9" s="3">
         <f t="shared" si="5"/>
-        <v>-55</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
         <v>5.6999999999999995E-2</v>
       </c>
-      <c r="N9">
-        <f>TRUNC(M9*4096,0)</f>
+      <c r="P9">
+        <f t="shared" si="6"/>
         <v>233</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D10" s="1"/>
       <c r="E10">
+        <f t="shared" si="7"/>
+        <v>120</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.108</v>
+      </c>
+      <c r="H10" s="1">
         <f t="shared" si="3"/>
-        <v>120</v>
-      </c>
-      <c r="F10">
-        <f>(E10-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>1800</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0.108</v>
-      </c>
-      <c r="H10" s="1">
+        <v>442</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="9"/>
+        <v>-50</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>0.06</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="1"/>
-        <v>442</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="L10">
+        <v>245</v>
+      </c>
+      <c r="O10" s="3">
         <f t="shared" si="5"/>
-        <v>-50</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="2"/>
         <v>0.06</v>
       </c>
-      <c r="N10">
-        <f>TRUNC(M10*4096,0)</f>
+      <c r="P10">
+        <f t="shared" si="6"/>
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D11" s="1"/>
       <c r="E11">
+        <f t="shared" si="7"/>
+        <v>135</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>1950</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.11699999999999999</v>
+      </c>
+      <c r="H11" s="1">
         <f t="shared" si="3"/>
-        <v>135</v>
-      </c>
-      <c r="F11">
-        <f>(E11-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>1950</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.11699999999999999</v>
-      </c>
-      <c r="H11" s="1">
+        <v>479</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="9"/>
+        <v>-45</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>6.3E-2</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="1"/>
-        <v>479</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-      <c r="L11">
+        <v>258</v>
+      </c>
+      <c r="O11" s="3">
         <f t="shared" si="5"/>
-        <v>-45</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
         <v>6.3E-2</v>
       </c>
-      <c r="N11">
-        <f>TRUNC(M11*4096,0)</f>
+      <c r="P11">
+        <f t="shared" si="6"/>
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D12" s="1"/>
       <c r="E12">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.126</v>
+      </c>
+      <c r="H12" s="1">
         <f t="shared" si="3"/>
-        <v>150</v>
-      </c>
-      <c r="F12">
-        <f>(E12-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>2100</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0.126</v>
-      </c>
-      <c r="H12" s="1">
+        <v>516</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="9"/>
+        <v>-40</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="1"/>
-        <v>516</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="L12">
+        <v>270</v>
+      </c>
+      <c r="O12" s="3">
         <f t="shared" si="5"/>
-        <v>-40</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="N12">
-        <f>TRUNC(M12*4096,0)</f>
+      <c r="P12">
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D13" s="1"/>
       <c r="E13">
+        <f t="shared" si="7"/>
+        <v>165</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.13499999999999998</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" si="3"/>
-        <v>165</v>
-      </c>
-      <c r="F13">
-        <f>(E13-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>2250</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0.13499999999999998</v>
-      </c>
-      <c r="H13" s="1">
+        <v>552</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="8"/>
+        <v>55</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="9"/>
+        <v>-35</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="1"/>
-        <v>552</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="4"/>
-        <v>55</v>
-      </c>
-      <c r="L13">
+        <v>282</v>
+      </c>
+      <c r="O13" s="3">
         <f t="shared" si="5"/>
-        <v>-35</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="2"/>
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="N13">
-        <f>TRUNC(M13*4096,0)</f>
+      <c r="P13">
+        <f t="shared" si="6"/>
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D14" s="1"/>
       <c r="E14">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="H14" s="1">
         <f t="shared" si="3"/>
-        <v>180</v>
-      </c>
-      <c r="F14">
-        <f>(E14-$B$1)*($B$4-$B$3)/($B$2-$B$1)+$B$3</f>
-        <v>2400</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="H14" s="1">
+        <v>589</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="9"/>
+        <v>-30</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>7.2000000000000008E-2</v>
+      </c>
+      <c r="N14">
         <f t="shared" si="1"/>
-        <v>589</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="L14">
+        <v>294</v>
+      </c>
+      <c r="O14" s="3">
         <f t="shared" si="5"/>
-        <v>-30</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
         <v>7.2000000000000008E-2</v>
       </c>
-      <c r="N14">
-        <f>TRUNC(M14*4096,0)</f>
+      <c r="P14">
+        <f t="shared" si="6"/>
         <v>294</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="I15" s="1"/>
       <c r="K15">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="9"/>
+        <v>-25</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="4"/>
-        <v>65</v>
-      </c>
-      <c r="L15">
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>307</v>
+      </c>
+      <c r="O15" s="3">
         <f t="shared" si="5"/>
-        <v>-25</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
         <v>7.5000000000000011E-2</v>
       </c>
-      <c r="N15">
-        <f>TRUNC(M15*4096,0)</f>
+      <c r="P15">
+        <f t="shared" si="6"/>
         <v>307</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="I16" s="1"/>
       <c r="K16">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="9"/>
+        <v>-20</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="4"/>
-        <v>70</v>
-      </c>
-      <c r="L16">
+        <v>7.7999999999999986E-2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>319</v>
+      </c>
+      <c r="O16" s="3">
         <f t="shared" si="5"/>
-        <v>-20</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
         <v>7.7999999999999986E-2</v>
       </c>
-      <c r="N16">
-        <f>TRUNC(M16*4096,0)</f>
+      <c r="P16">
+        <f t="shared" si="6"/>
         <v>319</v>
       </c>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="I17" s="1"/>
       <c r="K17">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="9"/>
+        <v>-15</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="4"/>
-        <v>75</v>
-      </c>
-      <c r="L17">
+        <v>8.0999999999999989E-2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>331</v>
+      </c>
+      <c r="O17" s="3">
         <f t="shared" si="5"/>
-        <v>-15</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="2"/>
         <v>8.0999999999999989E-2</v>
       </c>
-      <c r="N17">
-        <f>TRUNC(M17*4096,0)</f>
+      <c r="P17">
+        <f t="shared" si="6"/>
         <v>331</v>
       </c>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="I18" s="1"/>
       <c r="K18">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="9"/>
+        <v>-10</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="4"/>
-        <v>80</v>
-      </c>
-      <c r="L18">
+        <v>8.3999999999999991E-2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>344</v>
+      </c>
+      <c r="O18" s="3">
         <f t="shared" si="5"/>
-        <v>-10</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="2"/>
         <v>8.3999999999999991E-2</v>
       </c>
-      <c r="N18">
-        <f>TRUNC(M18*4096,0)</f>
+      <c r="P18">
+        <f t="shared" si="6"/>
         <v>344</v>
       </c>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="I19" s="1"/>
       <c r="K19">
+        <f t="shared" si="8"/>
+        <v>85</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="9"/>
+        <v>-5</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="4"/>
-        <v>85</v>
-      </c>
-      <c r="L19">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>356</v>
+      </c>
+      <c r="O19" s="3">
         <f t="shared" si="5"/>
-        <v>-5</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="2"/>
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="N19">
-        <f>TRUNC(M19*4096,0)</f>
+      <c r="P19">
+        <f t="shared" si="6"/>
         <v>356</v>
       </c>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="K20">
+        <f t="shared" si="8"/>
+        <v>90</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M20">
         <f t="shared" si="4"/>
-        <v>90</v>
-      </c>
-      <c r="L20">
+        <v>0.09</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>368</v>
+      </c>
+      <c r="O20" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="2"/>
         <v>0.09</v>
       </c>
-      <c r="N20">
-        <f>TRUNC(M20*4096,0)</f>
+      <c r="P20">
+        <f t="shared" si="6"/>
         <v>368</v>
       </c>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="K21">
+        <f t="shared" si="8"/>
+        <v>95</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="M21">
         <f t="shared" si="4"/>
-        <v>95</v>
-      </c>
-      <c r="L21">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>380</v>
+      </c>
+      <c r="O21" s="3">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="2"/>
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="N21">
-        <f>TRUNC(M21*4096,0)</f>
+      <c r="P21">
+        <f t="shared" si="6"/>
         <v>380</v>
       </c>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="K22">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="M22">
         <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="L22">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>393</v>
+      </c>
+      <c r="O22" s="3">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="2"/>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="N22">
-        <f>TRUNC(M22*4096,0)</f>
+      <c r="P22">
+        <f t="shared" si="6"/>
         <v>393</v>
       </c>
     </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="K23">
+        <f t="shared" si="8"/>
+        <v>105</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="M23">
         <f t="shared" si="4"/>
-        <v>105</v>
-      </c>
-      <c r="L23">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+      <c r="O23" s="3">
         <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="2"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="N23">
-        <f>TRUNC(M23*4096,0)</f>
+      <c r="P23">
+        <f t="shared" si="6"/>
         <v>405</v>
       </c>
     </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="K24">
+        <f t="shared" si="8"/>
+        <v>110</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+      <c r="M24">
         <f t="shared" si="4"/>
-        <v>110</v>
-      </c>
-      <c r="L24">
+        <v>0.10200000000000001</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>417</v>
+      </c>
+      <c r="O24" s="3">
         <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="2"/>
         <v>0.10200000000000001</v>
       </c>
-      <c r="N24">
-        <f>TRUNC(M24*4096,0)</f>
+      <c r="P24">
+        <f t="shared" si="6"/>
         <v>417</v>
       </c>
     </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="K25">
+        <f t="shared" si="8"/>
+        <v>115</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="4"/>
-        <v>115</v>
-      </c>
-      <c r="L25">
+        <v>0.10499999999999998</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>430</v>
+      </c>
+      <c r="O25" s="3">
         <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="2"/>
         <v>0.10499999999999998</v>
       </c>
-      <c r="N25">
-        <f>TRUNC(M25*4096,0)</f>
+      <c r="P25">
+        <f t="shared" si="6"/>
         <v>430</v>
       </c>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="K26">
+        <f t="shared" si="8"/>
+        <v>120</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="M26">
         <f t="shared" si="4"/>
-        <v>120</v>
-      </c>
-      <c r="L26">
+        <v>0.10799999999999998</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>442</v>
+      </c>
+      <c r="O26" s="3">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="2"/>
         <v>0.10799999999999998</v>
       </c>
-      <c r="N26">
-        <f>TRUNC(M26*4096,0)</f>
+      <c r="P26">
+        <f t="shared" si="6"/>
         <v>442</v>
       </c>
     </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="K27">
+        <f t="shared" si="8"/>
+        <v>125</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="9"/>
+        <v>35</v>
+      </c>
+      <c r="M27">
         <f t="shared" si="4"/>
-        <v>125</v>
-      </c>
-      <c r="L27">
+        <v>0.11099999999999999</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>454</v>
+      </c>
+      <c r="O27" s="3">
         <f t="shared" si="5"/>
-        <v>35</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="2"/>
         <v>0.11099999999999999</v>
       </c>
-      <c r="N27">
-        <f>TRUNC(M27*4096,0)</f>
+      <c r="P27">
+        <f t="shared" si="6"/>
         <v>454</v>
       </c>
     </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="K28">
+        <f t="shared" si="8"/>
+        <v>130</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="9"/>
+        <v>40</v>
+      </c>
+      <c r="M28">
         <f t="shared" si="4"/>
-        <v>130</v>
-      </c>
-      <c r="L28">
+        <v>0.11399999999999999</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>466</v>
+      </c>
+      <c r="O28" s="3">
         <f t="shared" si="5"/>
-        <v>40</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="2"/>
         <v>0.11399999999999999</v>
       </c>
-      <c r="N28">
-        <f>TRUNC(M28*4096,0)</f>
+      <c r="P28">
+        <f t="shared" si="6"/>
         <v>466</v>
       </c>
     </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="K29">
+        <f t="shared" si="8"/>
+        <v>135</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="9"/>
+        <v>45</v>
+      </c>
+      <c r="M29">
         <f t="shared" si="4"/>
-        <v>135</v>
-      </c>
-      <c r="L29">
+        <v>0.11699999999999999</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>479</v>
+      </c>
+      <c r="O29" s="3">
         <f t="shared" si="5"/>
-        <v>45</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="2"/>
         <v>0.11699999999999999</v>
       </c>
-      <c r="N29">
-        <f>TRUNC(M29*4096,0)</f>
+      <c r="P29">
+        <f t="shared" si="6"/>
         <v>479</v>
       </c>
     </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="K30">
+        <f t="shared" si="8"/>
+        <v>140</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="M30">
         <f t="shared" si="4"/>
-        <v>140</v>
-      </c>
-      <c r="L30">
+        <v>0.12</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>491</v>
+      </c>
+      <c r="O30" s="3">
         <f t="shared" si="5"/>
-        <v>50</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="N30">
-        <f>TRUNC(M30*4096,0)</f>
+      <c r="P30">
+        <f t="shared" si="6"/>
         <v>491</v>
       </c>
     </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="K31">
+        <f t="shared" si="8"/>
+        <v>145</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="9"/>
+        <v>55</v>
+      </c>
+      <c r="M31">
         <f t="shared" si="4"/>
-        <v>145</v>
-      </c>
-      <c r="L31">
+        <v>0.123</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>503</v>
+      </c>
+      <c r="O31" s="3">
         <f t="shared" si="5"/>
-        <v>55</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="2"/>
         <v>0.123</v>
       </c>
-      <c r="N31">
-        <f>TRUNC(M31*4096,0)</f>
+      <c r="P31">
+        <f t="shared" si="6"/>
         <v>503</v>
       </c>
     </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="K32">
+        <f t="shared" si="8"/>
+        <v>150</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="M32">
         <f t="shared" si="4"/>
-        <v>150</v>
-      </c>
-      <c r="L32">
+        <v>0.126</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>516</v>
+      </c>
+      <c r="O32" s="3">
         <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="2"/>
         <v>0.126</v>
       </c>
-      <c r="N32">
-        <f>TRUNC(M32*4096,0)</f>
+      <c r="P32">
+        <f t="shared" si="6"/>
         <v>516</v>
       </c>
     </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="K33">
+        <f t="shared" si="8"/>
+        <v>155</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="9"/>
+        <v>65</v>
+      </c>
+      <c r="M33">
         <f t="shared" si="4"/>
-        <v>155</v>
-      </c>
-      <c r="L33">
+        <v>0.129</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>528</v>
+      </c>
+      <c r="O33" s="3">
         <f t="shared" si="5"/>
-        <v>65</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="2"/>
         <v>0.129</v>
       </c>
-      <c r="N33">
-        <f>TRUNC(M33*4096,0)</f>
+      <c r="P33">
+        <f t="shared" si="6"/>
         <v>528</v>
       </c>
     </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="K34">
+        <f t="shared" si="8"/>
+        <v>160</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="9"/>
+        <v>70</v>
+      </c>
+      <c r="M34">
         <f t="shared" si="4"/>
-        <v>160</v>
-      </c>
-      <c r="L34">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>540</v>
+      </c>
+      <c r="O34" s="3">
         <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="2"/>
         <v>0.13200000000000001</v>
       </c>
-      <c r="N34">
-        <f>TRUNC(M34*4096,0)</f>
+      <c r="P34">
+        <f t="shared" si="6"/>
         <v>540</v>
       </c>
     </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="K35">
+        <f t="shared" si="8"/>
+        <v>165</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="9"/>
+        <v>75</v>
+      </c>
+      <c r="M35">
         <f t="shared" si="4"/>
-        <v>165</v>
-      </c>
-      <c r="L35">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>552</v>
+      </c>
+      <c r="O35" s="3">
         <f t="shared" si="5"/>
-        <v>75</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="2"/>
         <v>0.13500000000000001</v>
       </c>
-      <c r="N35">
-        <f>TRUNC(M35*4096,0)</f>
+      <c r="P35">
+        <f t="shared" si="6"/>
         <v>552</v>
       </c>
     </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="K36">
+        <f t="shared" si="8"/>
+        <v>170</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="M36">
         <f t="shared" si="4"/>
-        <v>170</v>
-      </c>
-      <c r="L36">
+        <v>0.13799999999999998</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>565</v>
+      </c>
+      <c r="O36" s="3">
         <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="2"/>
         <v>0.13799999999999998</v>
       </c>
-      <c r="N36">
-        <f>TRUNC(M36*4096,0)</f>
+      <c r="P36">
+        <f t="shared" si="6"/>
         <v>565</v>
       </c>
     </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="K37">
+        <f t="shared" si="8"/>
+        <v>175</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="9"/>
+        <v>85</v>
+      </c>
+      <c r="M37">
         <f t="shared" si="4"/>
-        <v>175</v>
-      </c>
-      <c r="L37">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>577</v>
+      </c>
+      <c r="O37" s="3">
         <f t="shared" si="5"/>
-        <v>85</v>
-      </c>
-      <c r="M37">
-        <f t="shared" si="2"/>
         <v>0.14099999999999999</v>
       </c>
-      <c r="N37">
-        <f>TRUNC(M37*4096,0)</f>
+      <c r="P37">
+        <f t="shared" si="6"/>
         <v>577</v>
       </c>
     </row>
-    <row r="38" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -4870,11 +5266,19 @@
         <v>90</v>
       </c>
       <c r="M38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.14399999999999999</v>
       </c>
       <c r="N38">
-        <f>TRUNC(M38*4096,0)</f>
+        <f t="shared" si="1"/>
+        <v>589</v>
+      </c>
+      <c r="O38" s="3">
+        <f t="shared" si="5"/>
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="6"/>
         <v>589</v>
       </c>
     </row>

</xml_diff>